<commit_message>
Changed excel headers and developing code
</commit_message>
<xml_diff>
--- a/IrmaMudThicknessComparisons.xlsx
+++ b/IrmaMudThicknessComparisons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lszczyrba/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lszczyrba/Project_3.6.3/HelloWorld/Irma_Sediment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02292314-3EB5-4441-BB20-BCC16221DBD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2704A133-4973-6848-95B3-32B2E7ADBB2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="460" windowWidth="26940" windowHeight="18940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3640" yWindow="460" windowWidth="26940" windowHeight="18860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,18 +42,6 @@
     <t>Station</t>
   </si>
   <si>
-    <t>Date 1</t>
-  </si>
-  <si>
-    <t>Date 2</t>
-  </si>
-  <si>
-    <t>Thickness at Date 1 (cm)</t>
-  </si>
-  <si>
-    <t>Thickness at Date 2 (cm)</t>
-  </si>
-  <si>
     <t>Lat</t>
   </si>
   <si>
@@ -403,6 +391,18 @@
   </si>
   <si>
     <t>WTZ</t>
+  </si>
+  <si>
+    <t>Thick1(cm)</t>
+  </si>
+  <si>
+    <t>Thick2(cm)</t>
+  </si>
+  <si>
+    <t>Date1</t>
+  </si>
+  <si>
+    <t>Date2</t>
   </si>
 </sst>
 </file>
@@ -753,8 +753,8 @@
   <dimension ref="A1:J128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,36 +780,36 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D2" s="4">
         <v>43056</v>
@@ -832,13 +832,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D3" s="4">
         <v>43056</v>
@@ -861,13 +861,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D4" s="4">
         <v>43056</v>
@@ -890,13 +890,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D5" s="4">
         <v>43056</v>
@@ -919,13 +919,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D6" s="4">
         <v>43056</v>
@@ -948,13 +948,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D7" s="4">
         <v>43056</v>
@@ -977,13 +977,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D8" s="4">
         <v>43056</v>
@@ -1006,13 +1006,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4">
         <v>43056</v>
@@ -1035,13 +1035,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D10" s="4">
         <v>43056</v>
@@ -1064,13 +1064,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D11" s="4">
         <v>43057</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D12" s="4">
         <v>43057</v>
@@ -1104,13 +1104,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D13" s="4">
         <v>43057</v>
@@ -1124,13 +1124,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D14" s="4">
         <v>43057</v>
@@ -1144,13 +1144,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D15" s="4">
         <v>43057</v>
@@ -1164,13 +1164,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D16" s="4">
         <v>43057</v>
@@ -1184,13 +1184,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D17" s="4">
         <v>43057</v>
@@ -1204,13 +1204,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D18" s="4">
         <v>43057</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D19" s="4">
         <v>43057</v>
@@ -1239,18 +1239,18 @@
         <v>43173</v>
       </c>
       <c r="F19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D20" s="4">
         <v>43057</v>
@@ -1264,13 +1264,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D21" s="4">
         <v>43057</v>
@@ -1279,18 +1279,18 @@
         <v>43173</v>
       </c>
       <c r="F21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D22" s="4">
         <v>43057</v>
@@ -1304,13 +1304,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D23" s="4">
         <v>43057</v>
@@ -1324,13 +1324,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D24" s="4">
         <v>43057</v>
@@ -1344,13 +1344,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D25" s="4">
         <v>43057</v>
@@ -1361,13 +1361,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D26" s="4">
         <v>43058</v>
@@ -1376,7 +1376,7 @@
         <v>43173</v>
       </c>
       <c r="F26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -1390,13 +1390,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D27" s="4">
         <v>43058</v>
@@ -1405,7 +1405,7 @@
         <v>43173</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1419,13 +1419,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D28" s="4">
         <v>43058</v>
@@ -1434,7 +1434,7 @@
         <v>43173</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D29" s="4">
         <v>43058</v>
@@ -1477,13 +1477,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D30" s="4">
         <v>43058</v>
@@ -1492,7 +1492,7 @@
         <v>43173</v>
       </c>
       <c r="F30" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1506,13 +1506,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D31" s="4">
         <v>43058</v>
@@ -1535,13 +1535,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D32" s="4">
         <v>43058</v>
@@ -1564,13 +1564,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D33" s="4">
         <v>43058</v>
@@ -1593,13 +1593,13 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D34" s="4">
         <v>43058</v>
@@ -1622,13 +1622,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D35" s="4">
         <v>43058</v>
@@ -1651,13 +1651,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D36" s="4">
         <v>43058</v>
@@ -1680,13 +1680,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D37" s="4">
         <v>43058</v>
@@ -1709,13 +1709,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D38" s="4">
         <v>43058</v>
@@ -1738,13 +1738,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D39" s="4">
         <v>43058</v>
@@ -1767,13 +1767,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D40" s="4">
         <v>43058</v>
@@ -1796,13 +1796,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D41" s="4">
         <v>43058</v>
@@ -1825,13 +1825,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D42" s="4">
         <v>43058</v>
@@ -1840,7 +1840,7 @@
         <v>43172</v>
       </c>
       <c r="F42" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G42">
         <v>4</v>
@@ -1852,18 +1852,18 @@
         <v>-81.596459999999993</v>
       </c>
       <c r="J42" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D43" s="4">
         <v>43058</v>
@@ -1872,7 +1872,7 @@
         <v>43172</v>
       </c>
       <c r="F43" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G43">
         <v>4</v>
@@ -1884,18 +1884,18 @@
         <v>-81.596459999999993</v>
       </c>
       <c r="J43" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D44" s="4">
         <v>43058</v>
@@ -1916,18 +1916,18 @@
         <v>-81.596410000000006</v>
       </c>
       <c r="J44" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D45" s="4">
         <v>43058</v>
@@ -1936,7 +1936,7 @@
         <v>43172</v>
       </c>
       <c r="F45" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G45">
         <v>2</v>
@@ -1948,18 +1948,18 @@
         <v>-81.596419999999995</v>
       </c>
       <c r="J45" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D46" s="4">
         <v>43058</v>
@@ -1980,18 +1980,18 @@
         <v>-81.596410000000006</v>
       </c>
       <c r="J46" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D47" s="4">
         <v>43058</v>
@@ -2012,18 +2012,18 @@
         <v>-81.59639</v>
       </c>
       <c r="J47" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D48" s="4">
         <v>43058</v>
@@ -2044,18 +2044,18 @@
         <v>-81.59639</v>
       </c>
       <c r="J48" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D49" s="4">
         <v>43058</v>
@@ -2076,18 +2076,18 @@
         <v>-81.596379999999996</v>
       </c>
       <c r="J49" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D50" s="4">
         <v>43058</v>
@@ -2108,18 +2108,18 @@
         <v>-81.569490000000002</v>
       </c>
       <c r="J50" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D51" s="4">
         <v>43058</v>
@@ -2140,18 +2140,18 @@
         <v>-81.596469999999997</v>
       </c>
       <c r="J51" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="D52" s="4">
         <v>43058</v>
@@ -2172,18 +2172,18 @@
         <v>-81.596450000000004</v>
       </c>
       <c r="J52" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D53" s="4">
         <v>43058</v>
@@ -2204,18 +2204,18 @@
         <v>-81.596419999999995</v>
       </c>
       <c r="J53" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D54" s="4">
         <v>43058</v>
@@ -2236,18 +2236,18 @@
         <v>-81.596369999999993</v>
       </c>
       <c r="J54" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D55" s="4">
         <v>43058</v>
@@ -2268,18 +2268,18 @@
         <v>-81.596310000000003</v>
       </c>
       <c r="J55" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D56" s="4">
         <v>43087</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C57" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D57" s="4">
         <v>43087</v>
@@ -2317,7 +2317,7 @@
         <v>43127</v>
       </c>
       <c r="F57" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G57">
         <v>0.5</v>
@@ -2331,13 +2331,13 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D58" s="4">
         <v>43087</v>
@@ -2360,13 +2360,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C59" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D59" s="4">
         <v>43087</v>
@@ -2389,13 +2389,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D60" s="4">
         <v>43087</v>
@@ -2404,7 +2404,7 @@
         <v>43127</v>
       </c>
       <c r="F60" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G60">
         <v>1.5</v>
@@ -2418,13 +2418,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D61" s="4">
         <v>43087</v>
@@ -2447,13 +2447,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D62" s="4">
         <v>43087</v>
@@ -2476,13 +2476,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C63" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D63" s="4">
         <v>43087</v>
@@ -2505,13 +2505,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D64" s="4">
         <v>43087</v>
@@ -2534,13 +2534,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D65" s="4">
         <v>43087</v>
@@ -2563,13 +2563,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C66" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D66" s="4">
         <v>43087</v>
@@ -2592,13 +2592,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D67" s="4">
         <v>43087</v>
@@ -2621,13 +2621,13 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C68" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D68" s="4">
         <v>43087</v>
@@ -2650,13 +2650,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C69" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D69" s="4">
         <v>43087</v>
@@ -2679,13 +2679,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C70" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D70" s="4">
         <v>43087</v>
@@ -2708,13 +2708,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C71" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D71" s="4">
         <v>43087</v>
@@ -2737,13 +2737,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C72" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D72" s="4">
         <v>43087</v>
@@ -2766,13 +2766,13 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" t="s">
         <v>67</v>
-      </c>
-      <c r="C73" t="s">
-        <v>71</v>
       </c>
       <c r="D73" s="4">
         <v>43087</v>
@@ -2795,13 +2795,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C74" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D74" s="4">
         <v>43087</v>
@@ -2824,13 +2824,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C75" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D75" s="4">
         <v>43087</v>
@@ -2853,32 +2853,32 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C76" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D76" s="4">
         <v>43087</v>
       </c>
       <c r="F76" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C77" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D77" s="4">
         <v>43087</v>
@@ -2891,13 +2891,13 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C78" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D78" s="4">
         <v>43087</v>
@@ -2910,13 +2910,13 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C79" t="s">
         <v>90</v>
-      </c>
-      <c r="C79" t="s">
-        <v>94</v>
       </c>
       <c r="D79" s="4">
         <v>43087</v>
@@ -2929,13 +2929,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C80" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D80" s="4">
         <v>43087</v>
@@ -2948,32 +2948,32 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C81" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D81" s="4">
         <v>43087</v>
       </c>
       <c r="F81" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C82" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D82" s="4">
         <v>43087</v>
@@ -2986,13 +2986,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C83" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D83" s="4">
         <v>43087</v>
@@ -3005,13 +3005,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C84" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D84" s="4">
         <v>43087</v>
@@ -3024,13 +3024,13 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C85" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D85" s="4">
         <v>43087</v>
@@ -3043,13 +3043,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D86" s="4">
         <v>43088</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D87" s="4">
         <v>43088</v>
@@ -3101,13 +3101,13 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D88" s="4">
         <v>43088</v>
@@ -3130,13 +3130,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D89" s="4">
         <v>43088</v>
@@ -3159,13 +3159,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D90" s="4">
         <v>43088</v>
@@ -3188,13 +3188,13 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D91" s="4">
         <v>43088</v>
@@ -3217,13 +3217,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D92" s="4">
         <v>43088</v>
@@ -3246,13 +3246,13 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D93" s="4">
         <v>43088</v>
@@ -3275,13 +3275,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D94" s="4">
         <v>43088</v>
@@ -3304,13 +3304,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D95" s="4">
         <v>43088</v>
@@ -3333,13 +3333,13 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D96" s="4">
         <v>43088</v>
@@ -3362,13 +3362,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D97" s="4">
         <v>43088</v>
@@ -3391,13 +3391,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D98" s="4">
         <v>43088</v>
@@ -3420,13 +3420,13 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D99" s="4">
         <v>43088</v>
@@ -3449,13 +3449,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D100" s="4">
         <v>43088</v>
@@ -3478,13 +3478,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D101" s="4">
         <v>43088</v>
@@ -3507,13 +3507,13 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D102" s="4">
         <v>43088</v>
@@ -3536,13 +3536,13 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D103" s="4">
         <v>43088</v>
@@ -3565,13 +3565,13 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D104" s="4">
         <v>43088</v>
@@ -3594,13 +3594,13 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D105" s="4">
         <v>43088</v>
@@ -3623,13 +3623,13 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D106" s="4">
         <v>43088</v>
@@ -3652,13 +3652,13 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D107" s="4">
         <v>43088</v>
@@ -3669,13 +3669,13 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D108" s="4">
         <v>43089</v>
@@ -3692,13 +3692,13 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D109" s="4">
         <v>43089</v>
@@ -3715,13 +3715,13 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D110" s="4">
         <v>43089</v>
@@ -3744,13 +3744,13 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D111" s="4">
         <v>43089</v>
@@ -3767,13 +3767,13 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D112" s="4">
         <v>43089</v>
@@ -3796,13 +3796,13 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D113" s="4">
         <v>43089</v>
@@ -3819,13 +3819,13 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D114" s="4">
         <v>43089</v>
@@ -3842,13 +3842,13 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D115" s="4">
         <v>43089</v>
@@ -3865,13 +3865,13 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D116" s="4">
         <v>43089</v>
@@ -3889,13 +3889,13 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D117" s="4">
         <v>43089</v>
@@ -3912,13 +3912,13 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D118" s="4">
         <v>43089</v>
@@ -3941,13 +3941,13 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D119" s="4">
         <v>43089</v>
@@ -3965,13 +3965,13 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4">
@@ -3989,13 +3989,13 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4">
@@ -4013,13 +4013,13 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4">
@@ -4037,13 +4037,13 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4">
@@ -4061,13 +4061,13 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4">
@@ -4085,13 +4085,13 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B125" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4">
@@ -4109,13 +4109,13 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>43</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4">
@@ -4133,13 +4133,13 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4">
@@ -4157,13 +4157,13 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4">

</xml_diff>